<commit_message>
Added orderTests and orderTestsStatusHistory API
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/donationInfo.xlsx
+++ b/BloodstreamAPI/testData/donationInfo.xlsx
@@ -3,17 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1F6D8F7C-D273-4506-8BA5-750F06DE53E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C83A2452-EFCE-4692-B371-38C670B8E632}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13395" windowHeight="9585" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12330" windowHeight="9585" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="donations" sheetId="2" r:id="rId1"/>
     <sheet name="donationShortDetail" sheetId="3" r:id="rId2"/>
     <sheet name="groupStatusCount" sheetId="4" r:id="rId3"/>
+    <sheet name="orderTests" sheetId="5" r:id="rId4"/>
+    <sheet name="orderTestsStatusHistory" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M29"/>
+  <oleSize ref="A1:L29"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="20">
   <si>
     <t>GroupStatus</t>
   </si>
@@ -74,6 +76,15 @@
   </si>
   <si>
     <t>/donationInfo/groupStatusCount</t>
+  </si>
+  <si>
+    <t>/donationInfo/orderTests</t>
+  </si>
+  <si>
+    <t>AA1</t>
+  </si>
+  <si>
+    <t>/donationInfo/orderTestStatusHistory</t>
   </si>
 </sst>
 </file>
@@ -631,7 +642,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E11"/>
+      <selection activeCell="E11" sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28A8DE7-7690-40F2-B6C7-91F96B21F039}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -880,6 +891,308 @@
       <c r="D11" s="4"/>
       <c r="E11" s="7" t="s">
         <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A9:E9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC63ECD6-8FDB-4F3A-A1DD-55CBC02E3453}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A9:E9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AB8C18-7D1C-4165-AD12-23B7B851E3F3}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>